<commit_message>
- move location ò 2 column {POS, CK}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_SoQuyNganHang.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_SoQuyNganHang.xlsx
@@ -271,14 +271,14 @@
     <xf numFmtId="3" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -588,7 +588,7 @@
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,27 +613,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-    </row>
-    <row r="2" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+    </row>
+    <row r="2" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
       <c r="B2" s="24"/>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -650,8 +650,8 @@
       <c r="O2" s="26"/>
       <c r="P2" s="26"/>
     </row>
-    <row r="3" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+    <row r="3" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
       <c r="B3" s="24"/>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -668,7 +668,7 @@
       <c r="O3" s="26"/>
       <c r="P3" s="26"/>
     </row>
-    <row r="4" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="25"/>
@@ -686,8 +686,8 @@
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
     </row>
-    <row r="5" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+    <row r="5" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
       <c r="B5" s="24"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
@@ -704,8 +704,8 @@
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
     </row>
-    <row r="6" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+    <row r="6" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
       <c r="B6" s="24"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -722,8 +722,8 @@
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
     </row>
-    <row r="7" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+    <row r="7" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
       <c r="B7" s="24"/>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
@@ -740,7 +740,7 @@
       <c r="O7" s="26"/>
       <c r="P7" s="26"/>
     </row>
-    <row r="8" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="27"/>
       <c r="C8" s="25"/>
@@ -779,10 +779,10 @@
         <v>6</v>
       </c>
       <c r="F10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>12</v>

</xml_diff>